<commit_message>
major dynamic roadmap changes
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/testdata.xlsx
+++ b/src/main/resources/testdata/testdata.xlsx
@@ -16,37 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>efg</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>operation</t>
   </si>
@@ -63,25 +33,58 @@
     <t>xpath</t>
   </si>
   <si>
-    <t>sdf</t>
-  </si>
-  <si>
-    <t>hgf</t>
-  </si>
-  <si>
-    <t>976g</t>
-  </si>
-  <si>
-    <t>5rs</t>
-  </si>
-  <si>
-    <t>ttr</t>
-  </si>
-  <si>
-    <t>//*[@id=\"maincontent\"]/div[2]/div/div[2]/div[1]/div[4]/div/a</t>
-  </si>
-  <si>
-    <t>//*[@id=\"send2\"]</t>
+    <t>//*[@id=\"firstname\"]</t>
+  </si>
+  <si>
+    <t>Automation 1</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Xpath</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>emailmaster@mailinator.com</t>
+  </si>
+  <si>
+    <t>Test@123</t>
+  </si>
+  <si>
+    <t>//*[@id="lastname"]</t>
+  </si>
+  <si>
+    <t>//*[@id="email_address"]</t>
+  </si>
+  <si>
+    <t>//*[@id="password"]</t>
+  </si>
+  <si>
+    <t>//*[@id="password-confirmation"]</t>
+  </si>
+  <si>
+    <t>//*[@id=\"gender\"]</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Sendkeys</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>Feature Step Name</t>
+  </si>
+  <si>
+    <t>fill_all_mandatory_fields</t>
   </si>
 </sst>
 </file>
@@ -427,111 +430,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.140625" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="67.140625" customWidth="1"/>
+    <col min="3" max="3" width="47.42578125" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <v>98</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D7" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -552,25 +560,25 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
50% dynamic completion done kindly check and merge
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/testdata.xlsx
+++ b/src/main/resources/testdata/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
   <si>
     <t>operation</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Action</t>
   </si>
   <si>
-    <t>Xpath</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -72,26 +69,110 @@
     <t>//*[@id=\"gender\"]</t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Sendkeys</t>
-  </si>
-  <si>
-    <t>Select</t>
-  </si>
-  <si>
     <t>Feature Step Name</t>
   </si>
   <si>
     <t>fill_all_mandatory_fields</t>
+  </si>
+  <si>
+    <t>dropdown_selection</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Clicks</t>
+  </si>
+  <si>
+    <t>Conditionclick</t>
+  </si>
+  <si>
+    <t>GetURL</t>
+  </si>
+  <si>
+    <t>scrolltoelem</t>
+  </si>
+  <si>
+    <t>formfill</t>
+  </si>
+  <si>
+    <t>Deselect</t>
+  </si>
+  <si>
+    <t>sleeper</t>
+  </si>
+  <si>
+    <t>explicitwait</t>
+  </si>
+  <si>
+    <t>implicitwait</t>
+  </si>
+  <si>
+    <t>methods</t>
+  </si>
+  <si>
+    <t>//*[@id=\"maincontent\"]/div[1]/h1/span</t>
+  </si>
+  <si>
+    <t>//*[@id=\"send2\"]/span</t>
+  </si>
+  <si>
+    <t>//*[@id=\"maincontent\"]/div[2]/div/div[2]/div[1]/div[4]/div/a/span</t>
+  </si>
+  <si>
+    <t>verify_page</t>
+  </si>
+  <si>
+    <t>No need</t>
+  </si>
+  <si>
+    <t>fill_other_fields</t>
+  </si>
+  <si>
+    <t>//*[@id=\"form-validate\"]/fieldset[1]/div[3]/div/button</t>
+  </si>
+  <si>
+    <t>//*[@id=\"ui-datepicker-div\"]/div[1]/div/select[1]</t>
+  </si>
+  <si>
+    <t>//*[@id=\"ui-datepicker-div\"]/div[1]/div/select[2]</t>
+  </si>
+  <si>
+    <t>//*[@id=\"ui-datepicker-div\"]/div[2]/button</t>
+  </si>
+  <si>
+    <t>//*[@id=\"form-validate\"]/fieldset[1]/div[8]/label/span/a</t>
+  </si>
+  <si>
+    <t>Xpath/cssSelector</t>
+  </si>
+  <si>
+    <t>check_checkbox_optional</t>
+  </si>
+  <si>
+    <t>no need</t>
+  </si>
+  <si>
+    <t>//*[@id=\"form-validate\"]/fieldset[1]/div[9]/label</t>
+  </si>
+  <si>
+    <t>div.field:nth-child(15) &gt; label:nth-child(2)</t>
+  </si>
+  <si>
+    <t>#consent_email_checkbox_label</t>
+  </si>
+  <si>
+    <t>#remember-me-box &gt; label:nth-child(2)</t>
+  </si>
+  <si>
+    <t>Apr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +183,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF17C6A3"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1EB540"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -126,9 +213,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,119 +518,336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="67.140625" customWidth="1"/>
-    <col min="3" max="3" width="47.42578125" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" customWidth="1"/>
+    <col min="3" max="3" width="62" customWidth="1"/>
     <col min="4" max="4" width="35.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
       <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1938</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>18</v>
-      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E16 B5:B11 B2:B3 B13:B17 B19:B22">
+      <formula1>$E$6:$E$16</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Please add and merge changes of feature files and other
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/testdata.xlsx
+++ b/src/main/resources/testdata/testdata.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sample.feature" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
   <si>
     <t>operation</t>
   </si>
@@ -166,13 +166,16 @@
   </si>
   <si>
     <t>Apr</t>
+  </si>
+  <si>
+    <t>Info</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,15 +185,35 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF17C6A3"/>
+      <color rgb="FF1EB540"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
-      <color rgb="FF1EB540"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -213,9 +236,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -518,334 +544,341 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" customWidth="1"/>
-    <col min="3" max="3" width="62" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="62" style="2" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="C13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1938</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E12" s="2" t="s">
+      <c r="C17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="C20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="2" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1938</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="C22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
+      <c r="B24" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E16 B5:B11 B2:B3 B13:B17 B19:B22">
-      <formula1>$E$6:$E$16</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F12 B5:B11 B2:B3 B13:B17 B19:B22">
+      <formula1>$F$2:$F$12</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
checkpoints nd new operation added
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/testdata.xlsx
+++ b/src/main/resources/testdata/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
   <si>
     <t>operation</t>
   </si>
@@ -169,6 +169,18 @@
   </si>
   <si>
     <t>Info</t>
+  </si>
+  <si>
+    <t>verifyText</t>
+  </si>
+  <si>
+    <t>//span[@class='base']</t>
+  </si>
+  <si>
+    <t>Create New Customer Account</t>
+  </si>
+  <si>
+    <t>hoverOn</t>
   </si>
 </sst>
 </file>
@@ -544,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,9 +605,6 @@
       <c r="D2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -610,14 +619,6 @@
       <c r="D3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -632,25 +633,19 @@
       <c r="D5" s="3">
         <v>5</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -661,13 +656,10 @@
         <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -678,13 +670,10 @@
         <v>25</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -695,13 +684,10 @@
         <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -712,13 +698,10 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -726,35 +709,27 @@
         <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F12" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -762,13 +737,13 @@
         <v>36</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -779,10 +754,10 @@
         <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="3">
-        <v>1938</v>
+        <v>38</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -790,13 +765,13 @@
         <v>36</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1938</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -804,44 +779,44 @@
         <v>36</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="2">
-        <v>5</v>
-      </c>
+      <c r="A19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="D20" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -852,7 +827,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>44</v>
@@ -863,64 +838,160 @@
         <v>43</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F12 B5:B11 B2:B3 B13:B17 B19:B22">
-      <formula1>$F$2:$F$12</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet2!$F$2:$F$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>B7:B12 B14:B18 B2:B3 B20:B22</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet2!$F$2:$F$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5:B6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet2!$F$2:$F$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>B23</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D5"/>
+  <dimension ref="A2:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F12">
+      <formula1>$F$2:$F$12</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+      <formula1>$F$2:$F$14</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
changes on path with dynamic
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/testdata.xlsx
+++ b/src/main/resources/testdata/testdata.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sample.feature" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="temp" sheetId="2" r:id="rId1"/>
+    <sheet name="Sample.feature" sheetId="1" r:id="rId2"/>
+    <sheet name="categories.feature" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="105">
   <si>
     <t>operation</t>
   </si>
@@ -181,13 +181,163 @@
   </si>
   <si>
     <t>hoverOn</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-id-3"]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-id-26"]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-id-51"]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-id-73"]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="ui-id-79"]/span</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Takescreenshot</t>
+  </si>
+  <si>
+    <t>take_screeshot_of_homepage</t>
+  </si>
+  <si>
+    <t>click_on_main_menu_content</t>
+  </si>
+  <si>
+    <t>//*[@id=\"wpn-lightbox-close-newsletter\"]</t>
+  </si>
+  <si>
+    <t>//*[@id=\"html-body\"]/aside/div/div/div[2]/button[1]</t>
+  </si>
+  <si>
+    <t>//span[text() = 'Shopping Cart']</t>
+  </si>
+  <si>
+    <t>//a[@href="https://vanssgstg.ada-asia.my/customer/account/login/" and text() = 'Sign In ']</t>
+  </si>
+  <si>
+    <t>//li/a[@href="https://vanssgstg.ada-asia.my/store-locator/" and text() = 'Find a Store']</t>
+  </si>
+  <si>
+    <t>//li/a[@href="https://vanssgstg.ada-asia.my/contact/"]</t>
+  </si>
+  <si>
+    <t>//a[@href="https://vanssgstg.ada-asia.my/specommerce/guest/wishlist/" and text() = 'Favourite        ']</t>
+  </si>
+  <si>
+    <t>https://vanssgstg.ada-asia.my/checkout/cart/</t>
+  </si>
+  <si>
+    <t>https://vanssgstg.ada-asia.my/specommerce/guest/wishlist/</t>
+  </si>
+  <si>
+    <t>https://vanssgstg.ada-asia.my/customer/account/login/</t>
+  </si>
+  <si>
+    <t>https://vanssgstg.ada-asia.my/store-locator/</t>
+  </si>
+  <si>
+    <t>Shoppting Page</t>
+  </si>
+  <si>
+    <t>Favourite Page</t>
+  </si>
+  <si>
+    <t>Sign In Page</t>
+  </si>
+  <si>
+    <t>Help Page</t>
+  </si>
+  <si>
+    <t>redirect_to_main_navigations</t>
+  </si>
+  <si>
+    <t>//a[@class='logo' and @href = 'https://vanssgstg.ada-asia.my/']</t>
+  </si>
+  <si>
+    <t>https://vanssgstg.ada-asia.my/contact/</t>
+  </si>
+  <si>
+    <t>Homepage</t>
+  </si>
+  <si>
+    <t>https://vanssgstg.ada-asia.my/</t>
+  </si>
+  <si>
+    <t>Store Locator</t>
+  </si>
+  <si>
+    <t>https://vanssgstg.ada-asia.my/new-arrivals.html</t>
+  </si>
+  <si>
+    <t>New Arrivals</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>https://vanssgstg.ada-asia.my/catalog/category/view/s/men/id/12/</t>
+  </si>
+  <si>
+    <t>//a[@id = 'ui-id-3']</t>
+  </si>
+  <si>
+    <t>//a[@id = 'ui-id-30']</t>
+  </si>
+  <si>
+    <t>//a[@id = 'ui-id-103']</t>
+  </si>
+  <si>
+    <t>//a[@id = 'ui-id-143']</t>
+  </si>
+  <si>
+    <t>//a[@id = 'ui-id-151']</t>
+  </si>
+  <si>
+    <t>//a[@id = 'ui-id-152']</t>
+  </si>
+  <si>
+    <t>//a[@id = 'ui-id-156']</t>
+  </si>
+  <si>
+    <t>Men</t>
+  </si>
+  <si>
+    <t>https://vanssgstg.ada-asia.my/catalog/category/view/s/women/id/21/</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>https://vanssgstg.ada-asia.my/catalog/category/view/s/kids/id/42/</t>
+  </si>
+  <si>
+    <t>Kids</t>
+  </si>
+  <si>
+    <t>https://vanssgstg.ada-asia.my/skate.html</t>
+  </si>
+  <si>
+    <t>Skate</t>
+  </si>
+  <si>
+    <t>mens</t>
+  </si>
+  <si>
+    <t>https://vanssgstg.ada-asia.my/mens-8206-3.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +377,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -245,18 +403,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -556,10 +717,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A2:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F12">
+      <formula1>$F$2:$F$12</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+      <formula1>$F$2:$F$14</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,32 +1128,119 @@
         <v>44</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
+      <c r="A25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Sheet2!$F$2:$F$12</xm:f>
+            <xm:f>temp!$F$2:$F$12</xm:f>
           </x14:formula1>
-          <xm:sqref>B7:B12 B14:B18 B2:B3 B20:B22</xm:sqref>
+          <xm:sqref>B7:B12 B14:B18 B20:B22 B3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Sheet2!$F$2:$F$13</xm:f>
+            <xm:f>temp!$F$2:$F$13</xm:f>
           </x14:formula1>
           <xm:sqref>B5:B6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Sheet2!$F$2:$F$14</xm:f>
+            <xm:f>temp!$F$2:$F$14</xm:f>
           </x14:formula1>
-          <xm:sqref>B23</xm:sqref>
+          <xm:sqref>B2 B23:B27 B29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>temp!$F$2:$F$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>B28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -894,115 +1248,801 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F14"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="68.5703125" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="F4" s="1" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F5" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F8" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F9" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F10" s="1" t="s">
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F11" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F12" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F13" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F14" s="1" t="s">
-        <v>54</v>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" t="s">
+        <v>87</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" t="s">
+        <v>93</v>
+      </c>
+      <c r="D48" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" t="s">
+        <v>87</v>
+      </c>
+      <c r="D51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" t="s">
+        <v>94</v>
+      </c>
+      <c r="D52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" t="s">
+        <v>87</v>
+      </c>
+      <c r="D54" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56" t="s">
+        <v>95</v>
+      </c>
+      <c r="D56" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F12">
-      <formula1>$F$2:$F$12</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
-      <formula1>$F$2:$F$14</formula1>
-    </dataValidation>
-  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D9" r:id="rId1"/>
+    <hyperlink ref="D13" r:id="rId2"/>
+    <hyperlink ref="D17" r:id="rId3"/>
+    <hyperlink ref="D21" r:id="rId4"/>
+    <hyperlink ref="D46" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>temp!$F$2:$F$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2 B4:B26 B28:B56</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes with extent reports
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/testdata.xlsx
+++ b/src/main/resources/testdata/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="106">
   <si>
     <t>operation</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>https://vanssgstg.ada-asia.my/mens-8206-3.html</t>
+  </si>
+  <si>
+    <t>Homescreen</t>
   </si>
 </sst>
 </file>
@@ -1252,8 +1255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1670,7 +1673,9 @@
       <c r="C31" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="6"/>
+      <c r="D31" s="6" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">

</xml_diff>

<commit_message>
Commit for few changes on data sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/testdata.xlsx
+++ b/src/main/resources/testdata/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="113">
   <si>
     <t>operation</t>
   </si>
@@ -213,9 +213,6 @@
     <t>//*[@id=\"wpn-lightbox-close-newsletter\"]</t>
   </si>
   <si>
-    <t>//*[@id=\"html-body\"]/aside/div/div/div[2]/button[1]</t>
-  </si>
-  <si>
     <t>//span[text() = 'Shopping Cart']</t>
   </si>
   <si>
@@ -342,9 +339,6 @@
     <t>Click on the newsletter</t>
   </si>
   <si>
-    <t>no issue</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -358,6 +352,9 @@
   </si>
   <si>
     <t xml:space="preserve">//a[@id = 'ui-id-156'] </t>
+  </si>
+  <si>
+    <t>//button[@class="amgdprcookie-button -allow -save" and text()="ACCEPT ALL"]</t>
   </si>
 </sst>
 </file>
@@ -1297,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,10 +1337,10 @@
         <v>35</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1360,7 +1357,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1377,7 +1374,7 @@
         <v>35</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1393,232 +1390,229 @@
       <c r="D6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C8" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="9" t="s">
+      <c r="D16" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="11">
+      <c r="C17" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B9" s="9" t="s">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="C18" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="9" t="s">
+      <c r="C19" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="C20" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="11">
+      <c r="C21" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="9" t="s">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="12" t="s">
+      <c r="C22" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1626,13 +1620,13 @@
         <v>63</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>35</v>
+        <v>35</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1640,444 +1634,444 @@
         <v>63</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="11">
+      <c r="C25" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="9" t="s">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="9" t="s">
+      <c r="C26" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>35</v>
+      <c r="C27" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="11">
-        <v>2</v>
+      <c r="D29" s="11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>83</v>
+      <c r="D30" s="11">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>87</v>
+        <v>35</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B33" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D33" s="11">
+      <c r="C34" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B34" s="9" t="s">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="C35" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B37" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C38" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" s="12" t="s">
         <v>87</v>
-      </c>
-      <c r="D37" s="11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B41" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D41" s="11">
+      <c r="C42" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B42" s="9" t="s">
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="C43" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B45" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D45" s="11">
+      <c r="C46" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B46" s="9" t="s">
+    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="C47" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>99</v>
+        <v>86</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B49" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C49" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D49" s="11">
+      <c r="C50" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B50" s="9" t="s">
+    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C50" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="C51" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B53" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C53" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D53" s="11">
+      <c r="C54" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D54" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B54" s="9" t="s">
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B55" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C54" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="C55" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D56" s="11" t="s">
         <v>109</v>
@@ -2085,41 +2079,41 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B57" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B58" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C57" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="D57" s="11">
+      <c r="C58" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D58" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B58" s="9" t="s">
+    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B59" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="C59" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D59" s="11" t="s">
         <v>102</v>
@@ -2127,26 +2121,40 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B60" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C60" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>87</v>
+      <c r="C61" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1"/>
-    <hyperlink ref="D13" r:id="rId2"/>
-    <hyperlink ref="D17" r:id="rId3"/>
-    <hyperlink ref="D21" r:id="rId4"/>
-    <hyperlink ref="D46" r:id="rId5"/>
-    <hyperlink ref="D54" r:id="rId6"/>
+    <hyperlink ref="D10" r:id="rId1"/>
+    <hyperlink ref="D14" r:id="rId2"/>
+    <hyperlink ref="D18" r:id="rId3"/>
+    <hyperlink ref="D22" r:id="rId4"/>
+    <hyperlink ref="D47" r:id="rId5"/>
+    <hyperlink ref="D55" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
@@ -2157,7 +2165,7 @@
           <x14:formula1>
             <xm:f>temp!$F$2:$F$15</xm:f>
           </x14:formula1>
-          <xm:sqref>B2 B4:B26 B28:B60</xm:sqref>
+          <xm:sqref>B2 B29:B61 B4:B27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Changes over 25 sept
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/testdata.xlsx
+++ b/src/main/resources/testdata/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="122">
   <si>
     <t>operation</t>
   </si>
@@ -355,6 +355,33 @@
   </si>
   <si>
     <t>//button[@class="amgdprcookie-button -allow -save" and text()="ACCEPT ALL"]</t>
+  </si>
+  <si>
+    <t>click_on_each_New_Arrival_Link</t>
+  </si>
+  <si>
+    <t>//a[@id='ui-id-5']</t>
+  </si>
+  <si>
+    <t>//a[@id='ui-id-7']</t>
+  </si>
+  <si>
+    <t>//a[@id='ui-id-8']</t>
+  </si>
+  <si>
+    <t>//a[@id='ui-id-9']</t>
+  </si>
+  <si>
+    <t>//a[@id='ui-id-10']</t>
+  </si>
+  <si>
+    <t>//a[@id='ui-id-12']</t>
+  </si>
+  <si>
+    <t>//a[@id='ui-id-11']</t>
+  </si>
+  <si>
+    <t>//a[@id='ui-id-14']</t>
   </si>
 </sst>
 </file>
@@ -1294,10 +1321,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,13 +1423,13 @@
         <v>63</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>35</v>
       </c>
       <c r="D7" s="11">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2144,6 +2171,440 @@
         <v>111</v>
       </c>
       <c r="D61" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D64" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D66" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D68" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D70" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D72" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D74" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D76" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D77" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D78" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D80" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D82" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D84" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D86" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D88" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C89" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C90" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D90" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D91" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D92" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D93" s="11" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2165,7 +2626,7 @@
           <x14:formula1>
             <xm:f>temp!$F$2:$F$15</xm:f>
           </x14:formula1>
-          <xm:sqref>B2 B29:B61 B4:B27</xm:sqref>
+          <xm:sqref>B2 B29:B61 B4:B27 B63:B93</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Long time now push it
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/testdata.xlsx
+++ b/src/main/resources/testdata/testdata.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="temp" sheetId="2" r:id="rId1"/>
     <sheet name="Sample.feature" sheetId="1" r:id="rId2"/>
     <sheet name="categories.feature" sheetId="3" r:id="rId3"/>
+    <sheet name="vansdemo.feature" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="138">
   <si>
     <t>operation</t>
   </si>
@@ -382,13 +383,61 @@
   </si>
   <si>
     <t>//a[@id='ui-id-14']</t>
+  </si>
+  <si>
+    <t>login_with_valid_username_and_password</t>
+  </si>
+  <si>
+    <t>//input[@id='a2.1.4.1:LoginField']</t>
+  </si>
+  <si>
+    <t>//input[@id='a2.1.4.1:Password']</t>
+  </si>
+  <si>
+    <t>karming.song@gmg.com</t>
+  </si>
+  <si>
+    <t>@Today123</t>
+  </si>
+  <si>
+    <t>Noneed</t>
+  </si>
+  <si>
+    <t>//*[@id="a2.1.4.1:LoginBtn"]/a</t>
+  </si>
+  <si>
+    <t>//button[@class='Primary iziToast-buttons-child' and text()='OK']</t>
+  </si>
+  <si>
+    <t>//a[@href='https://dam.vans.com/asset-management/2DBYOHERBY?WS=AssetManagement&amp;Flat=y']</t>
+  </si>
+  <si>
+    <t>go_to_catalogs</t>
+  </si>
+  <si>
+    <t>click_on_first_product</t>
+  </si>
+  <si>
+    <t>click_on_download_button</t>
+  </si>
+  <si>
+    <t>//a[@href='https://dam.vans.com/asset-management/2DBYOHH5I24K']</t>
+  </si>
+  <si>
+    <t>//a[@id="a3.5.1.1.1.1.4.6:2"]/a</t>
+  </si>
+  <si>
+    <t>//a[@role='button' and @aria-label='Standard download']</t>
+  </si>
+  <si>
+    <t>click_on_standard_download</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,6 +485,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -458,7 +513,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -486,6 +541,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1323,8 +1380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2632,4 +2689,335 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.5703125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="30" style="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="10">
+        <v>5</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="14">
+        <v>5</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="11">
+        <v>3</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="11">
+        <v>3</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" s="11">
+        <v>3</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="11">
+        <v>3</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" s="11">
+        <v>3</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="11">
+        <v>3</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="mailto:karming.song@gmg.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>temp!$F$2:$F$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B11 B13:B15 B17:B18 B20:B21</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>